<commit_message>
add materials for sessions 02
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/23-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9590AD-6F01-FF4D-B078-667B1092658C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530B569-DBB2-6E44-B164-923003C3F457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11200" yWindow="5900" windowWidth="28800" windowHeight="17500" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>week</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>prep/p02.html</t>
+  </si>
+  <si>
+    <t>prep/p03.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/session-02-the-mobile-connectivity-paradox-digital-wellbeing-as-a-dynamic-construct</t>
   </si>
 </sst>
 </file>
@@ -472,7 +478,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,6 +542,9 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
       <c r="G3" t="s">
         <v>15</v>
       </c>
@@ -549,6 +558,9 @@
       </c>
       <c r="C4" t="s">
         <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
add files for session 04
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fedietri/GitHub/23-1-nmok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BB706D-F75C-FD49-8F01-12C74CE7B4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307B7038-AFC5-E84A-B477-2D8887A43CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11200" yWindow="5900" windowWidth="28800" windowHeight="17500" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>week</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>prep/p04.html</t>
+  </si>
+  <si>
+    <t>exercises/e04.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/session-04-structuring-a-heterogeneous-field-the-basics-of-markdown-and-github</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,6 +594,12 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>

</xml_diff>